<commit_message>
Fixed Cashflow icon and window locaation on all tool builders
</commit_message>
<xml_diff>
--- a/My_application/third_party/PHPExcel/finance/test1.xlsx
+++ b/My_application/third_party/PHPExcel/finance/test1.xlsx
@@ -682,6 +682,60 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,61 +781,7 @@
     <xf numFmtId="44" fontId="14" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -807,6 +807,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2273300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>52870</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="476250"/>
+          <a:ext cx="2273300" cy="767245"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1078,7 +1121,7 @@
   <dimension ref="B1:H110"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1095,12 +1138,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
@@ -1110,18 +1153,18 @@
     </row>
     <row r="3" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -1137,8 +1180,8 @@
       <c r="F4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
@@ -1146,8 +1189,8 @@
       <c r="D5" s="12"/>
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
@@ -1159,19 +1202,19 @@
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="45">
-        <v>0</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="46">
-        <v>0</v>
-      </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47">
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40">
+        <v>0</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41">
         <f>+C7-E7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="47"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
@@ -1183,197 +1226,197 @@
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="39">
-        <v>0</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="40">
-        <v>0</v>
-      </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41">
+      <c r="C10" s="27">
+        <v>0</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="38">
         <f>+C10-E10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="41"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="39">
-        <v>0</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40">
-        <v>0</v>
-      </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41">
+      <c r="C11" s="27">
+        <v>0</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="38">
         <f t="shared" ref="G11:G18" si="0">+C11-E11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="41"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="39">
-        <v>0</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40">
-        <v>0</v>
-      </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41">
+      <c r="C12" s="27">
+        <v>0</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="41"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="39">
-        <v>0</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40">
-        <v>0</v>
-      </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="41">
+      <c r="C13" s="27">
+        <v>0</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28">
+        <v>0</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="41"/>
+      <c r="H13" s="38"/>
     </row>
     <row r="14" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="39">
-        <v>0</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40">
-        <v>0</v>
-      </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="41">
+      <c r="C14" s="27">
+        <v>0</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28">
+        <v>0</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="39">
-        <v>0</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40">
-        <v>0</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="41">
+      <c r="C15" s="27">
+        <v>0</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="41"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="39">
-        <v>0</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
-        <v>0</v>
-      </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41">
+      <c r="C16" s="27">
+        <v>0</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28">
+        <v>0</v>
+      </c>
+      <c r="F16" s="28"/>
+      <c r="G16" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="41"/>
+      <c r="H16" s="38"/>
     </row>
     <row r="17" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="39">
-        <v>0</v>
-      </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40">
-        <v>0</v>
-      </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="41">
+      <c r="C17" s="27">
+        <v>0</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28">
+        <v>0</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="41"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="42">
-        <v>0</v>
-      </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43">
-        <v>0</v>
-      </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44">
+      <c r="C18" s="30">
+        <v>0</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31">
+        <v>0</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="44"/>
+      <c r="H18" s="57"/>
     </row>
     <row r="19" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="54">
         <f>SUM(C10:D18)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36">
+      <c r="D19" s="54"/>
+      <c r="E19" s="54">
         <f>SUM(E10:F18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37">
+      <c r="F19" s="54"/>
+      <c r="G19" s="55">
         <f>+C19-E19</f>
         <v>0</v>
       </c>
-      <c r="H19" s="38"/>
+      <c r="H19" s="56"/>
     </row>
     <row r="20" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
@@ -1385,172 +1428,172 @@
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="51"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="22" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="39">
-        <v>0</v>
-      </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40">
-        <v>0</v>
-      </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="48">
+      <c r="C23" s="27">
+        <v>0</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28">
+        <v>0</v>
+      </c>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29">
         <f>+C23-E23</f>
         <v>0</v>
       </c>
-      <c r="H23" s="48"/>
+      <c r="H23" s="29"/>
     </row>
     <row r="24" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="39">
-        <v>0</v>
-      </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40">
-        <v>0</v>
-      </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="48">
+      <c r="C24" s="27">
+        <v>0</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28">
+        <v>0</v>
+      </c>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29">
         <f t="shared" ref="G24:G29" si="1">+C24-E24</f>
         <v>0</v>
       </c>
-      <c r="H24" s="48"/>
+      <c r="H24" s="29"/>
     </row>
     <row r="25" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="39">
-        <v>0</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40">
-        <v>0</v>
-      </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="48">
+      <c r="C25" s="27">
+        <v>0</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28">
+        <v>0</v>
+      </c>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H25" s="48"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="39">
-        <v>0</v>
-      </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="40">
-        <v>0</v>
-      </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="48">
+      <c r="C26" s="27">
+        <v>0</v>
+      </c>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28">
+        <v>0</v>
+      </c>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H26" s="48"/>
+      <c r="H26" s="29"/>
     </row>
     <row r="27" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="39">
-        <v>0</v>
-      </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40">
-        <v>0</v>
-      </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="48">
+      <c r="C27" s="27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28">
+        <v>0</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H27" s="48"/>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="39">
-        <v>0</v>
-      </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40">
-        <v>0</v>
-      </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="48">
+      <c r="C28" s="27">
+        <v>0</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H28" s="48"/>
+      <c r="H28" s="29"/>
     </row>
     <row r="29" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="42">
-        <v>0</v>
-      </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43">
-        <v>0</v>
-      </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="52">
+      <c r="C29" s="30">
+        <v>0</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31">
+        <v>0</v>
+      </c>
+      <c r="F29" s="31"/>
+      <c r="G29" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H29" s="52"/>
+      <c r="H29" s="32"/>
     </row>
     <row r="30" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="53">
+      <c r="C30" s="34">
         <f>SUM(C23:D29)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53">
+      <c r="D30" s="34"/>
+      <c r="E30" s="34">
         <f>SUM(E23:F29)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53">
+      <c r="F30" s="34"/>
+      <c r="G30" s="34">
         <f>+C30-E30</f>
         <v>0</v>
       </c>
-      <c r="H30" s="53"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
@@ -1562,539 +1605,539 @@
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="51"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
     </row>
     <row r="33" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="39">
-        <v>0</v>
-      </c>
-      <c r="D33" s="39"/>
-      <c r="E33" s="40">
-        <v>0</v>
-      </c>
-      <c r="F33" s="40"/>
-      <c r="G33" s="48">
+      <c r="C33" s="27">
+        <v>0</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28">
+        <v>0</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29">
         <f>+C33-E33</f>
         <v>0</v>
       </c>
-      <c r="H33" s="48"/>
+      <c r="H33" s="29"/>
     </row>
     <row r="34" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="39">
-        <v>0</v>
-      </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="40">
-        <v>0</v>
-      </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="48">
+      <c r="C34" s="27">
+        <v>0</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="28">
+        <v>0</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29">
         <f t="shared" ref="G34:G49" si="2">+C34-E34</f>
         <v>0</v>
       </c>
-      <c r="H34" s="48"/>
+      <c r="H34" s="29"/>
     </row>
     <row r="35" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="39">
-        <v>0</v>
-      </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="40">
-        <v>0</v>
-      </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="48">
+      <c r="C35" s="27">
+        <v>0</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28">
+        <v>0</v>
+      </c>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H35" s="48"/>
+      <c r="H35" s="29"/>
     </row>
     <row r="36" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="39">
-        <v>0</v>
-      </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="40">
-        <v>0</v>
-      </c>
-      <c r="F36" s="40"/>
-      <c r="G36" s="48">
+      <c r="C36" s="27">
+        <v>0</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28">
+        <v>0</v>
+      </c>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29">
         <f t="shared" ref="G36:G38" si="3">+C36-E36</f>
         <v>0</v>
       </c>
-      <c r="H36" s="48"/>
+      <c r="H36" s="29"/>
     </row>
     <row r="37" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="39">
-        <v>0</v>
-      </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="40">
-        <v>0</v>
-      </c>
-      <c r="F37" s="40"/>
-      <c r="G37" s="48">
+      <c r="C37" s="27">
+        <v>0</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="28">
+        <v>0</v>
+      </c>
+      <c r="F37" s="28"/>
+      <c r="G37" s="29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H37" s="48"/>
+      <c r="H37" s="29"/>
     </row>
     <row r="38" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="39">
-        <v>0</v>
-      </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="40">
-        <v>0</v>
-      </c>
-      <c r="F38" s="40"/>
-      <c r="G38" s="48">
+      <c r="C38" s="27">
+        <v>0</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="28">
+        <v>0</v>
+      </c>
+      <c r="F38" s="28"/>
+      <c r="G38" s="29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H38" s="48"/>
+      <c r="H38" s="29"/>
     </row>
     <row r="39" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="39">
-        <v>0</v>
-      </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="40">
-        <v>0</v>
-      </c>
-      <c r="F39" s="40"/>
-      <c r="G39" s="48">
+      <c r="C39" s="27">
+        <v>0</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="28">
+        <v>0</v>
+      </c>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29">
         <f>+C39-E39</f>
         <v>0</v>
       </c>
-      <c r="H39" s="48"/>
+      <c r="H39" s="29"/>
     </row>
     <row r="40" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="39">
-        <v>0</v>
-      </c>
-      <c r="D40" s="39"/>
-      <c r="E40" s="40">
-        <v>0</v>
-      </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="48">
+      <c r="C40" s="27">
+        <v>0</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="28">
+        <v>0</v>
+      </c>
+      <c r="F40" s="28"/>
+      <c r="G40" s="29">
         <f>+C40-E40</f>
         <v>0</v>
       </c>
-      <c r="H40" s="48"/>
+      <c r="H40" s="29"/>
     </row>
     <row r="41" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="39">
-        <v>0</v>
-      </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="40">
-        <v>0</v>
-      </c>
-      <c r="F41" s="40"/>
-      <c r="G41" s="48">
+      <c r="C41" s="27">
+        <v>0</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28">
+        <v>0</v>
+      </c>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29">
         <f>+C41-E41</f>
         <v>0</v>
       </c>
-      <c r="H41" s="48"/>
+      <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="39">
-        <v>0</v>
-      </c>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40">
-        <v>0</v>
-      </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="48">
+      <c r="C42" s="27">
+        <v>0</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="28">
+        <v>0</v>
+      </c>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29">
         <f t="shared" ref="G42:G46" si="4">+C42-E42</f>
         <v>0</v>
       </c>
-      <c r="H42" s="48"/>
+      <c r="H42" s="29"/>
     </row>
     <row r="43" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="39">
-        <v>0</v>
-      </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="40">
-        <v>0</v>
-      </c>
-      <c r="F43" s="40"/>
-      <c r="G43" s="48">
+      <c r="C43" s="27">
+        <v>0</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="28">
+        <v>0</v>
+      </c>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H43" s="48"/>
+      <c r="H43" s="29"/>
     </row>
     <row r="44" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="39">
-        <v>0</v>
-      </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="40">
-        <v>0</v>
-      </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="48">
+      <c r="C44" s="27">
+        <v>0</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="E44" s="28">
+        <v>0</v>
+      </c>
+      <c r="F44" s="28"/>
+      <c r="G44" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H44" s="48"/>
+      <c r="H44" s="29"/>
     </row>
     <row r="45" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="39">
-        <v>0</v>
-      </c>
-      <c r="D45" s="39"/>
-      <c r="E45" s="40">
-        <v>0</v>
-      </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="48">
+      <c r="C45" s="27">
+        <v>0</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28">
+        <v>0</v>
+      </c>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H45" s="48"/>
+      <c r="H45" s="29"/>
     </row>
     <row r="46" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="39">
-        <v>0</v>
-      </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="40">
-        <v>0</v>
-      </c>
-      <c r="F46" s="40"/>
-      <c r="G46" s="48">
+      <c r="C46" s="27">
+        <v>0</v>
+      </c>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28">
+        <v>0</v>
+      </c>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H46" s="48"/>
+      <c r="H46" s="29"/>
     </row>
     <row r="47" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="39">
-        <v>0</v>
-      </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="40">
-        <v>0</v>
-      </c>
-      <c r="F47" s="40"/>
-      <c r="G47" s="48">
+      <c r="C47" s="27">
+        <v>0</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28">
+        <v>0</v>
+      </c>
+      <c r="F47" s="28"/>
+      <c r="G47" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H47" s="48"/>
+      <c r="H47" s="29"/>
     </row>
     <row r="48" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="39">
-        <v>0</v>
-      </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="40">
-        <v>0</v>
-      </c>
-      <c r="F48" s="40"/>
-      <c r="G48" s="48">
+      <c r="C48" s="27">
+        <v>0</v>
+      </c>
+      <c r="D48" s="27"/>
+      <c r="E48" s="28">
+        <v>0</v>
+      </c>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H48" s="48"/>
+      <c r="H48" s="29"/>
     </row>
     <row r="49" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="39">
-        <v>0</v>
-      </c>
-      <c r="D49" s="39"/>
-      <c r="E49" s="40">
-        <v>0</v>
-      </c>
-      <c r="F49" s="40"/>
-      <c r="G49" s="48">
+      <c r="C49" s="27">
+        <v>0</v>
+      </c>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28">
+        <v>0</v>
+      </c>
+      <c r="F49" s="28"/>
+      <c r="G49" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H49" s="48"/>
+      <c r="H49" s="29"/>
     </row>
     <row r="50" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="39">
-        <v>0</v>
-      </c>
-      <c r="D50" s="39"/>
-      <c r="E50" s="40">
-        <v>0</v>
-      </c>
-      <c r="F50" s="40"/>
-      <c r="G50" s="48">
+      <c r="C50" s="27">
+        <v>0</v>
+      </c>
+      <c r="D50" s="27"/>
+      <c r="E50" s="28">
+        <v>0</v>
+      </c>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29">
         <f>+C50-E50</f>
         <v>0</v>
       </c>
-      <c r="H50" s="48"/>
+      <c r="H50" s="29"/>
     </row>
     <row r="51" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="39">
-        <v>0</v>
-      </c>
-      <c r="D51" s="39"/>
-      <c r="E51" s="40">
-        <v>0</v>
-      </c>
-      <c r="F51" s="40"/>
-      <c r="G51" s="48">
+      <c r="C51" s="27">
+        <v>0</v>
+      </c>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28">
+        <v>0</v>
+      </c>
+      <c r="F51" s="28"/>
+      <c r="G51" s="29">
         <f t="shared" ref="G51:G60" si="5">+C51-E51</f>
         <v>0</v>
       </c>
-      <c r="H51" s="48"/>
+      <c r="H51" s="29"/>
     </row>
     <row r="52" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="39">
-        <v>0</v>
-      </c>
-      <c r="D52" s="39"/>
-      <c r="E52" s="40">
-        <v>0</v>
-      </c>
-      <c r="F52" s="40"/>
-      <c r="G52" s="48">
+      <c r="C52" s="27">
+        <v>0</v>
+      </c>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28">
+        <v>0</v>
+      </c>
+      <c r="F52" s="28"/>
+      <c r="G52" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H52" s="48"/>
+      <c r="H52" s="29"/>
     </row>
     <row r="53" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="39">
-        <v>0</v>
-      </c>
-      <c r="D53" s="39"/>
-      <c r="E53" s="40">
-        <v>0</v>
-      </c>
-      <c r="F53" s="40"/>
-      <c r="G53" s="48">
+      <c r="C53" s="27">
+        <v>0</v>
+      </c>
+      <c r="D53" s="27"/>
+      <c r="E53" s="28">
+        <v>0</v>
+      </c>
+      <c r="F53" s="28"/>
+      <c r="G53" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H53" s="48"/>
+      <c r="H53" s="29"/>
     </row>
     <row r="54" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="39">
-        <v>0</v>
-      </c>
-      <c r="D54" s="39"/>
-      <c r="E54" s="40">
-        <v>0</v>
-      </c>
-      <c r="F54" s="40"/>
-      <c r="G54" s="48">
+      <c r="C54" s="27">
+        <v>0</v>
+      </c>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28">
+        <v>0</v>
+      </c>
+      <c r="F54" s="28"/>
+      <c r="G54" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H54" s="48"/>
+      <c r="H54" s="29"/>
     </row>
     <row r="55" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="39">
-        <v>0</v>
-      </c>
-      <c r="D55" s="39"/>
-      <c r="E55" s="40">
-        <v>0</v>
-      </c>
-      <c r="F55" s="40"/>
-      <c r="G55" s="48">
+      <c r="C55" s="27">
+        <v>0</v>
+      </c>
+      <c r="D55" s="27"/>
+      <c r="E55" s="28">
+        <v>0</v>
+      </c>
+      <c r="F55" s="28"/>
+      <c r="G55" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H55" s="48"/>
+      <c r="H55" s="29"/>
     </row>
     <row r="56" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="39">
-        <v>0</v>
-      </c>
-      <c r="D56" s="39"/>
-      <c r="E56" s="40">
-        <v>0</v>
-      </c>
-      <c r="F56" s="40"/>
-      <c r="G56" s="48">
+      <c r="C56" s="27">
+        <v>0</v>
+      </c>
+      <c r="D56" s="27"/>
+      <c r="E56" s="28">
+        <v>0</v>
+      </c>
+      <c r="F56" s="28"/>
+      <c r="G56" s="29">
         <f t="shared" ref="G56:G57" si="6">+C56-E56</f>
         <v>0</v>
       </c>
-      <c r="H56" s="48"/>
+      <c r="H56" s="29"/>
     </row>
     <row r="57" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="39">
-        <v>0</v>
-      </c>
-      <c r="D57" s="39"/>
-      <c r="E57" s="40">
-        <v>0</v>
-      </c>
-      <c r="F57" s="40"/>
-      <c r="G57" s="48">
+      <c r="C57" s="27">
+        <v>0</v>
+      </c>
+      <c r="D57" s="27"/>
+      <c r="E57" s="28">
+        <v>0</v>
+      </c>
+      <c r="F57" s="28"/>
+      <c r="G57" s="29">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H57" s="48"/>
+      <c r="H57" s="29"/>
     </row>
     <row r="58" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="39">
-        <v>0</v>
-      </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="40">
-        <v>0</v>
-      </c>
-      <c r="F58" s="40"/>
-      <c r="G58" s="48">
+      <c r="C58" s="27">
+        <v>0</v>
+      </c>
+      <c r="D58" s="27"/>
+      <c r="E58" s="28">
+        <v>0</v>
+      </c>
+      <c r="F58" s="28"/>
+      <c r="G58" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H58" s="48"/>
+      <c r="H58" s="29"/>
     </row>
     <row r="59" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="39">
-        <v>0</v>
-      </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="40">
-        <v>0</v>
-      </c>
-      <c r="F59" s="40"/>
-      <c r="G59" s="48">
+      <c r="C59" s="27">
+        <v>0</v>
+      </c>
+      <c r="D59" s="27"/>
+      <c r="E59" s="28">
+        <v>0</v>
+      </c>
+      <c r="F59" s="28"/>
+      <c r="G59" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H59" s="48"/>
+      <c r="H59" s="29"/>
     </row>
     <row r="60" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="42">
-        <v>0</v>
-      </c>
-      <c r="D60" s="42"/>
-      <c r="E60" s="43">
-        <v>0</v>
-      </c>
-      <c r="F60" s="43"/>
-      <c r="G60" s="52">
+      <c r="C60" s="30">
+        <v>0</v>
+      </c>
+      <c r="D60" s="30"/>
+      <c r="E60" s="31">
+        <v>0</v>
+      </c>
+      <c r="F60" s="31"/>
+      <c r="G60" s="32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H60" s="52"/>
+      <c r="H60" s="32"/>
     </row>
     <row r="61" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="53">
+      <c r="C61" s="34">
         <f>SUM(C33:D60)</f>
         <v>0</v>
       </c>
-      <c r="D61" s="53"/>
-      <c r="E61" s="53">
+      <c r="D61" s="34"/>
+      <c r="E61" s="34">
         <f>SUM(E33:F60)</f>
         <v>0</v>
       </c>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53">
+      <c r="F61" s="34"/>
+      <c r="G61" s="34">
         <f>+C61-E61</f>
         <v>0</v>
       </c>
-      <c r="H61" s="53"/>
+      <c r="H61" s="34"/>
     </row>
     <row r="62" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="6"/>
@@ -2106,161 +2149,161 @@
       <c r="H62" s="15"/>
     </row>
     <row r="63" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="49" t="s">
+      <c r="B63" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-      <c r="G63" s="50"/>
-      <c r="H63" s="51"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
     </row>
     <row r="64" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="39">
-        <v>0</v>
-      </c>
-      <c r="D64" s="39"/>
-      <c r="E64" s="40">
-        <v>0</v>
-      </c>
-      <c r="F64" s="40"/>
-      <c r="G64" s="48">
+      <c r="C64" s="27">
+        <v>0</v>
+      </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="28">
+        <v>0</v>
+      </c>
+      <c r="F64" s="28"/>
+      <c r="G64" s="29">
         <f>+C64-E64</f>
         <v>0</v>
       </c>
-      <c r="H64" s="48"/>
+      <c r="H64" s="29"/>
     </row>
     <row r="65" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="39">
-        <v>0</v>
-      </c>
-      <c r="D65" s="39"/>
-      <c r="E65" s="40">
-        <v>0</v>
-      </c>
-      <c r="F65" s="40"/>
-      <c r="G65" s="48">
+      <c r="C65" s="27">
+        <v>0</v>
+      </c>
+      <c r="D65" s="27"/>
+      <c r="E65" s="28">
+        <v>0</v>
+      </c>
+      <c r="F65" s="28"/>
+      <c r="G65" s="29">
         <f t="shared" ref="G65:G70" si="7">+C65-E65</f>
         <v>0</v>
       </c>
-      <c r="H65" s="48"/>
+      <c r="H65" s="29"/>
     </row>
     <row r="66" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="39">
-        <v>0</v>
-      </c>
-      <c r="D66" s="39"/>
-      <c r="E66" s="40">
-        <v>0</v>
-      </c>
-      <c r="F66" s="40"/>
-      <c r="G66" s="48">
+      <c r="C66" s="27">
+        <v>0</v>
+      </c>
+      <c r="D66" s="27"/>
+      <c r="E66" s="28">
+        <v>0</v>
+      </c>
+      <c r="F66" s="28"/>
+      <c r="G66" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H66" s="48"/>
+      <c r="H66" s="29"/>
     </row>
     <row r="67" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="39">
-        <v>0</v>
-      </c>
-      <c r="D67" s="39"/>
-      <c r="E67" s="40">
-        <v>0</v>
-      </c>
-      <c r="F67" s="40"/>
-      <c r="G67" s="48">
+      <c r="C67" s="27">
+        <v>0</v>
+      </c>
+      <c r="D67" s="27"/>
+      <c r="E67" s="28">
+        <v>0</v>
+      </c>
+      <c r="F67" s="28"/>
+      <c r="G67" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H67" s="48"/>
+      <c r="H67" s="29"/>
     </row>
     <row r="68" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="39">
-        <v>0</v>
-      </c>
-      <c r="D68" s="39"/>
-      <c r="E68" s="40">
-        <v>0</v>
-      </c>
-      <c r="F68" s="40"/>
-      <c r="G68" s="48">
+      <c r="C68" s="27">
+        <v>0</v>
+      </c>
+      <c r="D68" s="27"/>
+      <c r="E68" s="28">
+        <v>0</v>
+      </c>
+      <c r="F68" s="28"/>
+      <c r="G68" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H68" s="48"/>
+      <c r="H68" s="29"/>
     </row>
     <row r="69" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="39">
-        <v>0</v>
-      </c>
-      <c r="D69" s="39"/>
-      <c r="E69" s="40">
-        <v>0</v>
-      </c>
-      <c r="F69" s="40"/>
-      <c r="G69" s="48">
+      <c r="C69" s="27">
+        <v>0</v>
+      </c>
+      <c r="D69" s="27"/>
+      <c r="E69" s="28">
+        <v>0</v>
+      </c>
+      <c r="F69" s="28"/>
+      <c r="G69" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H69" s="48"/>
+      <c r="H69" s="29"/>
     </row>
     <row r="70" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="42">
-        <v>0</v>
-      </c>
-      <c r="D70" s="42"/>
-      <c r="E70" s="43">
-        <v>0</v>
-      </c>
-      <c r="F70" s="43"/>
-      <c r="G70" s="52">
+      <c r="C70" s="30">
+        <v>0</v>
+      </c>
+      <c r="D70" s="30"/>
+      <c r="E70" s="31">
+        <v>0</v>
+      </c>
+      <c r="F70" s="31"/>
+      <c r="G70" s="32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H70" s="52"/>
+      <c r="H70" s="32"/>
     </row>
     <row r="71" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C71" s="53">
+      <c r="C71" s="34">
         <f>SUM(C64:D70)</f>
         <v>0</v>
       </c>
-      <c r="D71" s="53"/>
-      <c r="E71" s="53">
+      <c r="D71" s="34"/>
+      <c r="E71" s="34">
         <f>SUM(E64:F70)</f>
         <v>0</v>
       </c>
-      <c r="F71" s="53"/>
-      <c r="G71" s="53">
+      <c r="F71" s="34"/>
+      <c r="G71" s="34">
         <f>+C71-E71</f>
         <v>0</v>
       </c>
-      <c r="H71" s="53"/>
+      <c r="H71" s="34"/>
     </row>
     <row r="72" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="6"/>
@@ -2275,21 +2318,21 @@
       <c r="B73" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C73" s="57">
+      <c r="C73" s="33">
         <f>SUM(C30,C61,C71)</f>
         <v>0</v>
       </c>
-      <c r="D73" s="57"/>
-      <c r="E73" s="57">
+      <c r="D73" s="33"/>
+      <c r="E73" s="33">
         <f>SUM(E30,E61,E71)</f>
         <v>0</v>
       </c>
-      <c r="F73" s="57"/>
-      <c r="G73" s="57">
+      <c r="F73" s="33"/>
+      <c r="G73" s="33">
         <f>+C73-E73</f>
         <v>0</v>
       </c>
-      <c r="H73" s="57"/>
+      <c r="H73" s="33"/>
     </row>
     <row r="74" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="6"/>
@@ -2304,21 +2347,21 @@
       <c r="B75" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="54">
+      <c r="C75" s="24">
         <f>C19-C73</f>
         <v>0</v>
       </c>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54">
+      <c r="D75" s="24"/>
+      <c r="E75" s="24">
         <f>E19-E73</f>
         <v>0</v>
       </c>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54">
+      <c r="F75" s="24"/>
+      <c r="G75" s="24">
         <f>+C75-E75</f>
         <v>0</v>
       </c>
-      <c r="H75" s="54"/>
+      <c r="H75" s="24"/>
     </row>
     <row r="76" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="6"/>
@@ -2333,21 +2376,21 @@
       <c r="B77" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C77" s="55">
+      <c r="C77" s="25">
         <f>SUM(C7,C19)-C73</f>
         <v>0</v>
       </c>
-      <c r="D77" s="55"/>
-      <c r="E77" s="56">
+      <c r="D77" s="25"/>
+      <c r="E77" s="26">
         <f>SUM(E7,E19)-E73</f>
         <v>0</v>
       </c>
-      <c r="F77" s="56"/>
-      <c r="G77" s="54">
+      <c r="F77" s="26"/>
+      <c r="G77" s="24">
         <f>+C77-E77</f>
         <v>0</v>
       </c>
-      <c r="H77" s="54"/>
+      <c r="H77" s="24"/>
     </row>
     <row r="78" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="16"/>
@@ -2648,6 +2691,168 @@
     </row>
   </sheetData>
   <mergeCells count="186">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H5"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="E75:F75"/>
     <mergeCell ref="G75:H75"/>
@@ -2672,170 +2877,9 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="G40:H40"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated File changes 7.0
</commit_message>
<xml_diff>
--- a/My_application/third_party/PHPExcel/finance/test1.xlsx
+++ b/My_application/third_party/PHPExcel/finance/test1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Simple Cash Flow Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>BEGIN</t>
   </si>
@@ -231,16 +231,19 @@
   <si>
     <t>PAYROLL BENEFITS - INDIRECT</t>
   </si>
+  <si>
+    <t>Currency</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +347,20 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -613,7 +630,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -682,37 +699,85 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="14" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="14" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,65 +789,29 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1121,7 +1150,7 @@
   <dimension ref="B1:H110"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1138,12 +1167,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="2:8" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
@@ -1153,18 +1186,18 @@
     </row>
     <row r="3" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="42" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="45"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -1180,8 +1213,8 @@
       <c r="F4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
@@ -1189,8 +1222,8 @@
       <c r="D5" s="12"/>
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
@@ -1202,19 +1235,19 @@
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="39">
-        <v>0</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40">
-        <v>0</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="41">
+      <c r="C7" s="47">
+        <v>0</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48">
+        <v>0</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="G7" s="49">
         <f>+C7-E7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="41"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
@@ -1226,197 +1259,197 @@
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="53"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="27">
-        <v>0</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28">
-        <v>0</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="38">
+      <c r="C10" s="41">
+        <v>0</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43">
         <f>+C10-E10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="38"/>
+      <c r="H10" s="43"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27">
-        <v>0</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28">
-        <v>0</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="38">
+      <c r="C11" s="41">
+        <v>0</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="43">
         <f t="shared" ref="G11:G18" si="0">+C11-E11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27">
-        <v>0</v>
-      </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28">
-        <v>0</v>
-      </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="38">
+      <c r="C12" s="41">
+        <v>0</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="27">
-        <v>0</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28">
-        <v>0</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="38">
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="38"/>
+      <c r="H13" s="43"/>
     </row>
     <row r="14" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="27">
-        <v>0</v>
-      </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28">
-        <v>0</v>
-      </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="38">
+      <c r="C14" s="41">
+        <v>0</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42">
+        <v>0</v>
+      </c>
+      <c r="F14" s="42"/>
+      <c r="G14" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="38"/>
+      <c r="H14" s="43"/>
     </row>
     <row r="15" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="27">
-        <v>0</v>
-      </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28">
-        <v>0</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="38">
+      <c r="C15" s="41">
+        <v>0</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="38"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="27">
-        <v>0</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28">
-        <v>0</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="38">
+      <c r="C16" s="41">
+        <v>0</v>
+      </c>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42">
+        <v>0</v>
+      </c>
+      <c r="F16" s="42"/>
+      <c r="G16" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="38"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="27">
-        <v>0</v>
-      </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28">
-        <v>0</v>
-      </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="38">
+      <c r="C17" s="41">
+        <v>0</v>
+      </c>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42">
+        <v>0</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="38"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="30">
-        <v>0</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31">
-        <v>0</v>
-      </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="57">
+      <c r="C18" s="44">
+        <v>0</v>
+      </c>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45">
+        <v>0</v>
+      </c>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="57"/>
+      <c r="H18" s="46"/>
     </row>
     <row r="19" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="38">
         <f>SUM(C10:D18)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54">
+      <c r="D19" s="38"/>
+      <c r="E19" s="38">
         <f>SUM(E10:F18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="55">
+      <c r="F19" s="38"/>
+      <c r="G19" s="39">
         <f>+C19-E19</f>
         <v>0</v>
       </c>
-      <c r="H19" s="56"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
@@ -1428,172 +1461,172 @@
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="37"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
     </row>
     <row r="22" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="27">
-        <v>0</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28">
-        <v>0</v>
-      </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29">
+      <c r="C23" s="41">
+        <v>0</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42">
+        <v>0</v>
+      </c>
+      <c r="F23" s="42"/>
+      <c r="G23" s="50">
         <f>+C23-E23</f>
         <v>0</v>
       </c>
-      <c r="H23" s="29"/>
+      <c r="H23" s="50"/>
     </row>
     <row r="24" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="27">
-        <v>0</v>
-      </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28">
-        <v>0</v>
-      </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29">
+      <c r="C24" s="41">
+        <v>0</v>
+      </c>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42">
+        <v>0</v>
+      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="50">
         <f t="shared" ref="G24:G29" si="1">+C24-E24</f>
         <v>0</v>
       </c>
-      <c r="H24" s="29"/>
+      <c r="H24" s="50"/>
     </row>
     <row r="25" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="27">
-        <v>0</v>
-      </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28">
-        <v>0</v>
-      </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29">
+      <c r="C25" s="41">
+        <v>0</v>
+      </c>
+      <c r="D25" s="41"/>
+      <c r="E25" s="42">
+        <v>0</v>
+      </c>
+      <c r="F25" s="42"/>
+      <c r="G25" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H25" s="29"/>
+      <c r="H25" s="50"/>
     </row>
     <row r="26" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="27">
-        <v>0</v>
-      </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28">
-        <v>0</v>
-      </c>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29">
+      <c r="C26" s="41">
+        <v>0</v>
+      </c>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42">
+        <v>0</v>
+      </c>
+      <c r="F26" s="42"/>
+      <c r="G26" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H26" s="29"/>
+      <c r="H26" s="50"/>
     </row>
     <row r="27" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="27">
-        <v>0</v>
-      </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28">
-        <v>0</v>
-      </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="29">
+      <c r="C27" s="41">
+        <v>0</v>
+      </c>
+      <c r="D27" s="41"/>
+      <c r="E27" s="42">
+        <v>0</v>
+      </c>
+      <c r="F27" s="42"/>
+      <c r="G27" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H27" s="29"/>
+      <c r="H27" s="50"/>
     </row>
     <row r="28" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="27">
-        <v>0</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29">
+      <c r="C28" s="41">
+        <v>0</v>
+      </c>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42">
+        <v>0</v>
+      </c>
+      <c r="F28" s="42"/>
+      <c r="G28" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H28" s="29"/>
+      <c r="H28" s="50"/>
     </row>
     <row r="29" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="30">
-        <v>0</v>
-      </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31">
-        <v>0</v>
-      </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="32">
+      <c r="C29" s="44">
+        <v>0</v>
+      </c>
+      <c r="D29" s="44"/>
+      <c r="E29" s="45">
+        <v>0</v>
+      </c>
+      <c r="F29" s="45"/>
+      <c r="G29" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H29" s="32"/>
+      <c r="H29" s="54"/>
     </row>
     <row r="30" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="55">
         <f>SUM(C23:D29)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34">
+      <c r="D30" s="55"/>
+      <c r="E30" s="55">
         <f>SUM(E23:F29)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34">
+      <c r="F30" s="55"/>
+      <c r="G30" s="55">
         <f>+C30-E30</f>
         <v>0</v>
       </c>
-      <c r="H30" s="34"/>
+      <c r="H30" s="55"/>
     </row>
     <row r="31" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
@@ -1605,539 +1638,539 @@
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
     </row>
     <row r="33" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="27">
-        <v>0</v>
-      </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28">
-        <v>0</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="29">
+      <c r="C33" s="41">
+        <v>0</v>
+      </c>
+      <c r="D33" s="41"/>
+      <c r="E33" s="42">
+        <v>0</v>
+      </c>
+      <c r="F33" s="42"/>
+      <c r="G33" s="50">
         <f>+C33-E33</f>
         <v>0</v>
       </c>
-      <c r="H33" s="29"/>
+      <c r="H33" s="50"/>
     </row>
     <row r="34" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="27">
-        <v>0</v>
-      </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="28">
-        <v>0</v>
-      </c>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29">
+      <c r="C34" s="41">
+        <v>0</v>
+      </c>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42">
+        <v>0</v>
+      </c>
+      <c r="F34" s="42"/>
+      <c r="G34" s="50">
         <f t="shared" ref="G34:G49" si="2">+C34-E34</f>
         <v>0</v>
       </c>
-      <c r="H34" s="29"/>
+      <c r="H34" s="50"/>
     </row>
     <row r="35" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="27">
-        <v>0</v>
-      </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28">
-        <v>0</v>
-      </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29">
+      <c r="C35" s="41">
+        <v>0</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42">
+        <v>0</v>
+      </c>
+      <c r="F35" s="42"/>
+      <c r="G35" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H35" s="29"/>
+      <c r="H35" s="50"/>
     </row>
     <row r="36" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="27">
-        <v>0</v>
-      </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="28">
-        <v>0</v>
-      </c>
-      <c r="F36" s="28"/>
-      <c r="G36" s="29">
+      <c r="C36" s="41">
+        <v>0</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42">
+        <v>0</v>
+      </c>
+      <c r="F36" s="42"/>
+      <c r="G36" s="50">
         <f t="shared" ref="G36:G38" si="3">+C36-E36</f>
         <v>0</v>
       </c>
-      <c r="H36" s="29"/>
+      <c r="H36" s="50"/>
     </row>
     <row r="37" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="27">
-        <v>0</v>
-      </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="28">
-        <v>0</v>
-      </c>
-      <c r="F37" s="28"/>
-      <c r="G37" s="29">
+      <c r="C37" s="41">
+        <v>0</v>
+      </c>
+      <c r="D37" s="41"/>
+      <c r="E37" s="42">
+        <v>0</v>
+      </c>
+      <c r="F37" s="42"/>
+      <c r="G37" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H37" s="29"/>
+      <c r="H37" s="50"/>
     </row>
     <row r="38" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="27">
-        <v>0</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="28">
-        <v>0</v>
-      </c>
-      <c r="F38" s="28"/>
-      <c r="G38" s="29">
+      <c r="C38" s="41">
+        <v>0</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42">
+        <v>0</v>
+      </c>
+      <c r="F38" s="42"/>
+      <c r="G38" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H38" s="29"/>
+      <c r="H38" s="50"/>
     </row>
     <row r="39" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="27">
-        <v>0</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="28">
-        <v>0</v>
-      </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="29">
+      <c r="C39" s="41">
+        <v>0</v>
+      </c>
+      <c r="D39" s="41"/>
+      <c r="E39" s="42">
+        <v>0</v>
+      </c>
+      <c r="F39" s="42"/>
+      <c r="G39" s="50">
         <f>+C39-E39</f>
         <v>0</v>
       </c>
-      <c r="H39" s="29"/>
+      <c r="H39" s="50"/>
     </row>
     <row r="40" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="27">
-        <v>0</v>
-      </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="28">
-        <v>0</v>
-      </c>
-      <c r="F40" s="28"/>
-      <c r="G40" s="29">
+      <c r="C40" s="41">
+        <v>0</v>
+      </c>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42">
+        <v>0</v>
+      </c>
+      <c r="F40" s="42"/>
+      <c r="G40" s="50">
         <f>+C40-E40</f>
         <v>0</v>
       </c>
-      <c r="H40" s="29"/>
+      <c r="H40" s="50"/>
     </row>
     <row r="41" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="27">
-        <v>0</v>
-      </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="28">
-        <v>0</v>
-      </c>
-      <c r="F41" s="28"/>
-      <c r="G41" s="29">
+      <c r="C41" s="41">
+        <v>0</v>
+      </c>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42">
+        <v>0</v>
+      </c>
+      <c r="F41" s="42"/>
+      <c r="G41" s="50">
         <f>+C41-E41</f>
         <v>0</v>
       </c>
-      <c r="H41" s="29"/>
+      <c r="H41" s="50"/>
     </row>
     <row r="42" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="27">
-        <v>0</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28">
-        <v>0</v>
-      </c>
-      <c r="F42" s="28"/>
-      <c r="G42" s="29">
+      <c r="C42" s="41">
+        <v>0</v>
+      </c>
+      <c r="D42" s="41"/>
+      <c r="E42" s="42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="42"/>
+      <c r="G42" s="50">
         <f t="shared" ref="G42:G46" si="4">+C42-E42</f>
         <v>0</v>
       </c>
-      <c r="H42" s="29"/>
+      <c r="H42" s="50"/>
     </row>
     <row r="43" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="27">
-        <v>0</v>
-      </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="28">
-        <v>0</v>
-      </c>
-      <c r="F43" s="28"/>
-      <c r="G43" s="29">
+      <c r="C43" s="41">
+        <v>0</v>
+      </c>
+      <c r="D43" s="41"/>
+      <c r="E43" s="42">
+        <v>0</v>
+      </c>
+      <c r="F43" s="42"/>
+      <c r="G43" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H43" s="29"/>
+      <c r="H43" s="50"/>
     </row>
     <row r="44" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="27">
-        <v>0</v>
-      </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="28">
-        <v>0</v>
-      </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="29">
+      <c r="C44" s="41">
+        <v>0</v>
+      </c>
+      <c r="D44" s="41"/>
+      <c r="E44" s="42">
+        <v>0</v>
+      </c>
+      <c r="F44" s="42"/>
+      <c r="G44" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H44" s="29"/>
+      <c r="H44" s="50"/>
     </row>
     <row r="45" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="27">
-        <v>0</v>
-      </c>
-      <c r="D45" s="27"/>
-      <c r="E45" s="28">
-        <v>0</v>
-      </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="29">
+      <c r="C45" s="41">
+        <v>0</v>
+      </c>
+      <c r="D45" s="41"/>
+      <c r="E45" s="42">
+        <v>0</v>
+      </c>
+      <c r="F45" s="42"/>
+      <c r="G45" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H45" s="29"/>
+      <c r="H45" s="50"/>
     </row>
     <row r="46" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="27">
-        <v>0</v>
-      </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="28">
-        <v>0</v>
-      </c>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29">
+      <c r="C46" s="41">
+        <v>0</v>
+      </c>
+      <c r="D46" s="41"/>
+      <c r="E46" s="42">
+        <v>0</v>
+      </c>
+      <c r="F46" s="42"/>
+      <c r="G46" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H46" s="29"/>
+      <c r="H46" s="50"/>
     </row>
     <row r="47" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="27">
-        <v>0</v>
-      </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="28">
-        <v>0</v>
-      </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="29">
+      <c r="C47" s="41">
+        <v>0</v>
+      </c>
+      <c r="D47" s="41"/>
+      <c r="E47" s="42">
+        <v>0</v>
+      </c>
+      <c r="F47" s="42"/>
+      <c r="G47" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H47" s="29"/>
+      <c r="H47" s="50"/>
     </row>
     <row r="48" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="27">
-        <v>0</v>
-      </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="28">
-        <v>0</v>
-      </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29">
+      <c r="C48" s="41">
+        <v>0</v>
+      </c>
+      <c r="D48" s="41"/>
+      <c r="E48" s="42">
+        <v>0</v>
+      </c>
+      <c r="F48" s="42"/>
+      <c r="G48" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H48" s="29"/>
+      <c r="H48" s="50"/>
     </row>
     <row r="49" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="27">
-        <v>0</v>
-      </c>
-      <c r="D49" s="27"/>
-      <c r="E49" s="28">
-        <v>0</v>
-      </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="29">
+      <c r="C49" s="41">
+        <v>0</v>
+      </c>
+      <c r="D49" s="41"/>
+      <c r="E49" s="42">
+        <v>0</v>
+      </c>
+      <c r="F49" s="42"/>
+      <c r="G49" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H49" s="29"/>
+      <c r="H49" s="50"/>
     </row>
     <row r="50" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="27">
-        <v>0</v>
-      </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="28">
-        <v>0</v>
-      </c>
-      <c r="F50" s="28"/>
-      <c r="G50" s="29">
+      <c r="C50" s="41">
+        <v>0</v>
+      </c>
+      <c r="D50" s="41"/>
+      <c r="E50" s="42">
+        <v>0</v>
+      </c>
+      <c r="F50" s="42"/>
+      <c r="G50" s="50">
         <f>+C50-E50</f>
         <v>0</v>
       </c>
-      <c r="H50" s="29"/>
+      <c r="H50" s="50"/>
     </row>
     <row r="51" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="27">
-        <v>0</v>
-      </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="28">
-        <v>0</v>
-      </c>
-      <c r="F51" s="28"/>
-      <c r="G51" s="29">
+      <c r="C51" s="41">
+        <v>0</v>
+      </c>
+      <c r="D51" s="41"/>
+      <c r="E51" s="42">
+        <v>0</v>
+      </c>
+      <c r="F51" s="42"/>
+      <c r="G51" s="50">
         <f t="shared" ref="G51:G60" si="5">+C51-E51</f>
         <v>0</v>
       </c>
-      <c r="H51" s="29"/>
+      <c r="H51" s="50"/>
     </row>
     <row r="52" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="27">
-        <v>0</v>
-      </c>
-      <c r="D52" s="27"/>
-      <c r="E52" s="28">
-        <v>0</v>
-      </c>
-      <c r="F52" s="28"/>
-      <c r="G52" s="29">
+      <c r="C52" s="41">
+        <v>0</v>
+      </c>
+      <c r="D52" s="41"/>
+      <c r="E52" s="42">
+        <v>0</v>
+      </c>
+      <c r="F52" s="42"/>
+      <c r="G52" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H52" s="29"/>
+      <c r="H52" s="50"/>
     </row>
     <row r="53" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="27">
-        <v>0</v>
-      </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="28">
-        <v>0</v>
-      </c>
-      <c r="F53" s="28"/>
-      <c r="G53" s="29">
+      <c r="C53" s="41">
+        <v>0</v>
+      </c>
+      <c r="D53" s="41"/>
+      <c r="E53" s="42">
+        <v>0</v>
+      </c>
+      <c r="F53" s="42"/>
+      <c r="G53" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H53" s="29"/>
+      <c r="H53" s="50"/>
     </row>
     <row r="54" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="27">
-        <v>0</v>
-      </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="28">
-        <v>0</v>
-      </c>
-      <c r="F54" s="28"/>
-      <c r="G54" s="29">
+      <c r="C54" s="41">
+        <v>0</v>
+      </c>
+      <c r="D54" s="41"/>
+      <c r="E54" s="42">
+        <v>0</v>
+      </c>
+      <c r="F54" s="42"/>
+      <c r="G54" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H54" s="29"/>
+      <c r="H54" s="50"/>
     </row>
     <row r="55" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="27">
-        <v>0</v>
-      </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="28">
-        <v>0</v>
-      </c>
-      <c r="F55" s="28"/>
-      <c r="G55" s="29">
+      <c r="C55" s="41">
+        <v>0</v>
+      </c>
+      <c r="D55" s="41"/>
+      <c r="E55" s="42">
+        <v>0</v>
+      </c>
+      <c r="F55" s="42"/>
+      <c r="G55" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H55" s="29"/>
+      <c r="H55" s="50"/>
     </row>
     <row r="56" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="27">
-        <v>0</v>
-      </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="28">
-        <v>0</v>
-      </c>
-      <c r="F56" s="28"/>
-      <c r="G56" s="29">
+      <c r="C56" s="41">
+        <v>0</v>
+      </c>
+      <c r="D56" s="41"/>
+      <c r="E56" s="42">
+        <v>0</v>
+      </c>
+      <c r="F56" s="42"/>
+      <c r="G56" s="50">
         <f t="shared" ref="G56:G57" si="6">+C56-E56</f>
         <v>0</v>
       </c>
-      <c r="H56" s="29"/>
+      <c r="H56" s="50"/>
     </row>
     <row r="57" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="27">
-        <v>0</v>
-      </c>
-      <c r="D57" s="27"/>
-      <c r="E57" s="28">
-        <v>0</v>
-      </c>
-      <c r="F57" s="28"/>
-      <c r="G57" s="29">
+      <c r="C57" s="41">
+        <v>0</v>
+      </c>
+      <c r="D57" s="41"/>
+      <c r="E57" s="42">
+        <v>0</v>
+      </c>
+      <c r="F57" s="42"/>
+      <c r="G57" s="50">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H57" s="29"/>
+      <c r="H57" s="50"/>
     </row>
     <row r="58" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="27">
-        <v>0</v>
-      </c>
-      <c r="D58" s="27"/>
-      <c r="E58" s="28">
-        <v>0</v>
-      </c>
-      <c r="F58" s="28"/>
-      <c r="G58" s="29">
+      <c r="C58" s="41">
+        <v>0</v>
+      </c>
+      <c r="D58" s="41"/>
+      <c r="E58" s="42">
+        <v>0</v>
+      </c>
+      <c r="F58" s="42"/>
+      <c r="G58" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H58" s="29"/>
+      <c r="H58" s="50"/>
     </row>
     <row r="59" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="27">
-        <v>0</v>
-      </c>
-      <c r="D59" s="27"/>
-      <c r="E59" s="28">
-        <v>0</v>
-      </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="29">
+      <c r="C59" s="41">
+        <v>0</v>
+      </c>
+      <c r="D59" s="41"/>
+      <c r="E59" s="42">
+        <v>0</v>
+      </c>
+      <c r="F59" s="42"/>
+      <c r="G59" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H59" s="29"/>
+      <c r="H59" s="50"/>
     </row>
     <row r="60" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="30">
-        <v>0</v>
-      </c>
-      <c r="D60" s="30"/>
-      <c r="E60" s="31">
-        <v>0</v>
-      </c>
-      <c r="F60" s="31"/>
-      <c r="G60" s="32">
+      <c r="C60" s="44">
+        <v>0</v>
+      </c>
+      <c r="D60" s="44"/>
+      <c r="E60" s="45">
+        <v>0</v>
+      </c>
+      <c r="F60" s="45"/>
+      <c r="G60" s="54">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H60" s="32"/>
+      <c r="H60" s="54"/>
     </row>
     <row r="61" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="34">
+      <c r="C61" s="55">
         <f>SUM(C33:D60)</f>
         <v>0</v>
       </c>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34">
+      <c r="D61" s="55"/>
+      <c r="E61" s="55">
         <f>SUM(E33:F60)</f>
         <v>0</v>
       </c>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34">
+      <c r="F61" s="55"/>
+      <c r="G61" s="55">
         <f>+C61-E61</f>
         <v>0</v>
       </c>
-      <c r="H61" s="34"/>
+      <c r="H61" s="55"/>
     </row>
     <row r="62" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="6"/>
@@ -2149,161 +2182,161 @@
       <c r="H62" s="15"/>
     </row>
     <row r="63" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="35" t="s">
+      <c r="B63" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="37"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="53"/>
     </row>
     <row r="64" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="27">
-        <v>0</v>
-      </c>
-      <c r="D64" s="27"/>
-      <c r="E64" s="28">
-        <v>0</v>
-      </c>
-      <c r="F64" s="28"/>
-      <c r="G64" s="29">
+      <c r="C64" s="41">
+        <v>0</v>
+      </c>
+      <c r="D64" s="41"/>
+      <c r="E64" s="42">
+        <v>0</v>
+      </c>
+      <c r="F64" s="42"/>
+      <c r="G64" s="50">
         <f>+C64-E64</f>
         <v>0</v>
       </c>
-      <c r="H64" s="29"/>
+      <c r="H64" s="50"/>
     </row>
     <row r="65" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="27">
-        <v>0</v>
-      </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="28">
-        <v>0</v>
-      </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29">
+      <c r="C65" s="41">
+        <v>0</v>
+      </c>
+      <c r="D65" s="41"/>
+      <c r="E65" s="42">
+        <v>0</v>
+      </c>
+      <c r="F65" s="42"/>
+      <c r="G65" s="50">
         <f t="shared" ref="G65:G70" si="7">+C65-E65</f>
         <v>0</v>
       </c>
-      <c r="H65" s="29"/>
+      <c r="H65" s="50"/>
     </row>
     <row r="66" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C66" s="27">
-        <v>0</v>
-      </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="28">
-        <v>0</v>
-      </c>
-      <c r="F66" s="28"/>
-      <c r="G66" s="29">
+      <c r="C66" s="41">
+        <v>0</v>
+      </c>
+      <c r="D66" s="41"/>
+      <c r="E66" s="42">
+        <v>0</v>
+      </c>
+      <c r="F66" s="42"/>
+      <c r="G66" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H66" s="29"/>
+      <c r="H66" s="50"/>
     </row>
     <row r="67" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="27">
-        <v>0</v>
-      </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="28">
-        <v>0</v>
-      </c>
-      <c r="F67" s="28"/>
-      <c r="G67" s="29">
+      <c r="C67" s="41">
+        <v>0</v>
+      </c>
+      <c r="D67" s="41"/>
+      <c r="E67" s="42">
+        <v>0</v>
+      </c>
+      <c r="F67" s="42"/>
+      <c r="G67" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H67" s="29"/>
+      <c r="H67" s="50"/>
     </row>
     <row r="68" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="27">
-        <v>0</v>
-      </c>
-      <c r="D68" s="27"/>
-      <c r="E68" s="28">
-        <v>0</v>
-      </c>
-      <c r="F68" s="28"/>
-      <c r="G68" s="29">
+      <c r="C68" s="41">
+        <v>0</v>
+      </c>
+      <c r="D68" s="41"/>
+      <c r="E68" s="42">
+        <v>0</v>
+      </c>
+      <c r="F68" s="42"/>
+      <c r="G68" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H68" s="29"/>
+      <c r="H68" s="50"/>
     </row>
     <row r="69" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="27">
-        <v>0</v>
-      </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="28">
-        <v>0</v>
-      </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="29">
+      <c r="C69" s="41">
+        <v>0</v>
+      </c>
+      <c r="D69" s="41"/>
+      <c r="E69" s="42">
+        <v>0</v>
+      </c>
+      <c r="F69" s="42"/>
+      <c r="G69" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H69" s="29"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="30">
-        <v>0</v>
-      </c>
-      <c r="D70" s="30"/>
-      <c r="E70" s="31">
-        <v>0</v>
-      </c>
-      <c r="F70" s="31"/>
-      <c r="G70" s="32">
+      <c r="C70" s="44">
+        <v>0</v>
+      </c>
+      <c r="D70" s="44"/>
+      <c r="E70" s="45">
+        <v>0</v>
+      </c>
+      <c r="F70" s="45"/>
+      <c r="G70" s="54">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H70" s="32"/>
+      <c r="H70" s="54"/>
     </row>
     <row r="71" spans="2:8" s="3" customFormat="1" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C71" s="34">
+      <c r="C71" s="55">
         <f>SUM(C64:D70)</f>
         <v>0</v>
       </c>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34">
+      <c r="D71" s="55"/>
+      <c r="E71" s="55">
         <f>SUM(E64:F70)</f>
         <v>0</v>
       </c>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34">
+      <c r="F71" s="55"/>
+      <c r="G71" s="55">
         <f>+C71-E71</f>
         <v>0</v>
       </c>
-      <c r="H71" s="34"/>
+      <c r="H71" s="55"/>
     </row>
     <row r="72" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="6"/>
@@ -2318,79 +2351,79 @@
       <c r="B73" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C73" s="33">
+      <c r="C73" s="59">
         <f>SUM(C30,C61,C71)</f>
         <v>0</v>
       </c>
-      <c r="D73" s="33"/>
-      <c r="E73" s="33">
+      <c r="D73" s="59"/>
+      <c r="E73" s="59">
         <f>SUM(E30,E61,E71)</f>
         <v>0</v>
       </c>
-      <c r="F73" s="33"/>
-      <c r="G73" s="33">
+      <c r="F73" s="59"/>
+      <c r="G73" s="59">
         <f>+C73-E73</f>
         <v>0</v>
       </c>
-      <c r="H73" s="33"/>
+      <c r="H73" s="59"/>
     </row>
     <row r="74" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="6"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
-      <c r="H74" s="15"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="25"/>
     </row>
     <row r="75" spans="2:8" s="13" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="24">
+      <c r="C75" s="56">
         <f>C19-C73</f>
         <v>0</v>
       </c>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24">
+      <c r="D75" s="56"/>
+      <c r="E75" s="56">
         <f>E19-E73</f>
         <v>0</v>
       </c>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24">
+      <c r="F75" s="56"/>
+      <c r="G75" s="56">
         <f>+C75-E75</f>
         <v>0</v>
       </c>
-      <c r="H75" s="24"/>
+      <c r="H75" s="56"/>
     </row>
     <row r="76" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="6"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
-      <c r="H76" s="15"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="25"/>
+      <c r="H76" s="25"/>
     </row>
     <row r="77" spans="2:8" s="13" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C77" s="25">
+      <c r="C77" s="57">
         <f>SUM(C7,C19)-C73</f>
         <v>0</v>
       </c>
-      <c r="D77" s="25"/>
-      <c r="E77" s="26">
+      <c r="D77" s="57"/>
+      <c r="E77" s="58">
         <f>SUM(E7,E19)-E73</f>
         <v>0</v>
       </c>
-      <c r="F77" s="26"/>
-      <c r="G77" s="24">
+      <c r="F77" s="58"/>
+      <c r="G77" s="56">
         <f>+C77-E77</f>
         <v>0</v>
       </c>
-      <c r="H77" s="24"/>
+      <c r="H77" s="56"/>
     </row>
     <row r="78" spans="2:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="16"/>
@@ -2691,6 +2724,168 @@
     </row>
   </sheetData>
   <mergeCells count="186">
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H5"/>
@@ -2715,171 +2910,9 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>